<commit_message>
Working version - February 8th, 2022
</commit_message>
<xml_diff>
--- a/Spreadsheets/Food Lists.xlsx
+++ b/Spreadsheets/Food Lists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwin365-my.sharepoint.com/personal/faverog_uwindsor_ca/Documents/Recipe Management/Spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="8_{A38D2D29-C639-4E0B-AE6F-A392D1526D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7ED6F60-922A-4ABE-90D6-9D48F33E8EFA}"/>
+  <xr:revisionPtr revIDLastSave="126" documentId="8_{A38D2D29-C639-4E0B-AE6F-A392D1526D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE8B52DB-4889-4D1C-91A2-6B5E2297DD5C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="3" xr2:uid="{E8E9E789-1EE6-4C1C-89B0-25405B9C8836}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{E8E9E789-1EE6-4C1C-89B0-25405B9C8836}"/>
   </bookViews>
   <sheets>
     <sheet name="Pastas" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Ricotta and Brocolli</t>
   </si>
@@ -63,9 +63,6 @@
     <t>American Steak</t>
   </si>
   <si>
-    <t>Frozen Pizza</t>
-  </si>
-  <si>
     <t>One Up One Down</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
   </si>
   <si>
     <t>Peas, Eggs &amp; Onion</t>
-  </si>
-  <si>
-    <t>Chicken Nuggets</t>
   </si>
   <si>
     <t>Salad</t>
@@ -477,7 +471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A6BB52-D52A-45AF-9CF1-F7BD4F56752B}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -491,7 +485,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -518,17 +512,17 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -552,7 +546,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
@@ -583,10 +577,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036E04D0-3406-4948-8ABD-4B8666D3767E}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -596,37 +590,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -638,7 +622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BFD1C36-4FAA-4A86-A4D7-755D0C075BCE}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -649,33 +633,33 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>